<commit_message>
stop using gh actions, rerender main figs
</commit_message>
<xml_diff>
--- a/analysis/manuscript/revision1/periphera.xlsx
+++ b/analysis/manuscript/revision1/periphera.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renatadiaz/Documents/GitHub/scadsanalysis/analysis/manuscript/revision1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56A5242-C298-6E4B-A524-0FAA31B35DF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49129D9E-802C-1D43-91D5-B14950434068}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24520" yWindow="1580" windowWidth="14040" windowHeight="20460" xr2:uid="{06609052-86CC-8D42-AA98-A109BF8CFAD6}"/>
+    <workbookView xWindow="24520" yWindow="1580" windowWidth="14040" windowHeight="20460" activeTab="1" xr2:uid="{06609052-86CC-8D42-AA98-A109BF8CFAD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Refs" sheetId="1" r:id="rId1"/>
@@ -688,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55112613-F84E-A74A-9C84-4D284AB61266}">
   <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1587,7 +1587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA86CEA-203E-DD48-A6D5-78FD9FC4A538}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>

</xml_diff>